<commit_message>
Updated after Production Run 2, Start of Production Run 3
</commit_message>
<xml_diff>
--- a/Production/Build Book/Word Clock BACK Jan24 KO/BOM Word Clock Gizmo BACK Jan24.xlsx
+++ b/Production/Build Book/Word Clock BACK Jan24 KO/BOM Word Clock Gizmo BACK Jan24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14kob\Downloads\gizmo-kyle-updateJan24\gizmo-kyle-updateJan24\Production\Build Book\Word Clock BACK Jan24 KO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brennan.reamer\Documents\gizmo\Production\Build Book\Word Clock BACK Jan24 KO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227D677B-CE4A-4F20-A833-B1C9F2DE599D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E4656D-B727-471B-B4CE-66F2E13017DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019-09-05 MicroWordClock2(Word" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
   <si>
     <t>Reference Designator</t>
   </si>
@@ -168,12 +168,6 @@
     <t>https://www.alibaba.com/product-detail/small-USB-shielded-high-speed-2_62016105964.html?spm=a2700.galleryofferlist.normalList.41.77cb4116Gb5sJX&amp;s=p</t>
   </si>
   <si>
-    <t>USB Block</t>
-  </si>
-  <si>
-    <t>https://www.alibaba.com/product-detail/1A-5V-Wall-Charger-Plug-USB_62093347466.html?spm=a2700.7724857.normalList.160.7ac27788RCl43u</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -273,31 +267,25 @@
     <t>Shenzhen Hezhongxin Electronics Co., Ltd</t>
   </si>
   <si>
-    <t>Guangzhou YHQ Trading Co., Ltd.</t>
-  </si>
-  <si>
     <t>Link (Old)</t>
   </si>
   <si>
-    <t>1A/5V Wall Plug</t>
-  </si>
-  <si>
     <t>Alternate Part Requested, requirements: ~90CM, Black, USB-A Male &lt;&gt; Micro-USB Male, Low-Cost</t>
   </si>
   <si>
-    <t>Alternate Part Requested, requirements: Black, 1A / 5V Wall Plug, EU (Type C) Plug to USB-A Female</t>
-  </si>
-  <si>
     <t>Real-Time Clock &amp; Battery</t>
   </si>
   <si>
     <t>Installed in J4/J5/J6/J7 during assembly.</t>
   </si>
   <si>
-    <t>Alternate Part Requested, requirements: DS3231 RTC, 4 Female Pin With Battery. Do Not Assemble; Pack &amp; Ship Separately.</t>
-  </si>
-  <si>
     <t>REF FILE 'RTC CANDIDATES'</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/HiLetgo-DS3231-Precision-Arduino-Raspberry/dp/B01N1LZSK3</t>
+  </si>
+  <si>
+    <t>Can use same as last production, requirements: DS3231 RTC, 4 Female Pin With Battery. Please assemble onto PCB (unlike last production)</t>
   </si>
 </sst>
 </file>
@@ -783,22 +771,22 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" style="21" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" style="23" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="124.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="14.42578125" style="9"/>
+    <col min="1" max="1" width="34.33203125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="42.88671875" style="21" customWidth="1"/>
+    <col min="3" max="3" width="43.5546875" style="23" customWidth="1"/>
+    <col min="4" max="4" width="39.88671875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="124.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="14.44140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" ht="14.25">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="13.8">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -806,22 +794,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="185.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="179.4">
       <c r="A2" s="28" t="s">
         <v>37</v>
       </c>
@@ -829,10 +817,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>4</v>
@@ -842,7 +830,7 @@
       </c>
       <c r="G2" s="17"/>
     </row>
-    <row r="3" spans="1:7" ht="14.25">
+    <row r="3" spans="1:7" ht="13.8">
       <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
@@ -850,10 +838,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>7</v>
@@ -863,7 +851,7 @@
       </c>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="1:7" ht="14.25">
+    <row r="4" spans="1:7" ht="13.8">
       <c r="A4" s="27" t="s">
         <v>8</v>
       </c>
@@ -871,10 +859,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>10</v>
@@ -884,7 +872,7 @@
       </c>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:7" ht="14.25">
+    <row r="5" spans="1:7" ht="13.8">
       <c r="A5" s="27" t="s">
         <v>11</v>
       </c>
@@ -892,10 +880,10 @@
         <v>12</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>13</v>
@@ -905,7 +893,7 @@
       </c>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:7" ht="14.25">
+    <row r="6" spans="1:7" ht="13.8">
       <c r="A6" s="27" t="s">
         <v>14</v>
       </c>
@@ -913,41 +901,41 @@
         <v>15</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:7" ht="14.25">
+    <row r="7" spans="1:7" ht="13.8">
       <c r="A7" s="29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="2">
         <v>4</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="14.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="13.8">
       <c r="A8" s="27" t="s">
         <v>17</v>
       </c>
@@ -955,10 +943,10 @@
         <v>18</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>19</v>
@@ -968,7 +956,7 @@
       </c>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" ht="14.25">
+    <row r="9" spans="1:7" ht="13.8">
       <c r="A9" s="15" t="s">
         <v>20</v>
       </c>
@@ -976,10 +964,10 @@
         <v>39</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>40</v>
@@ -989,7 +977,7 @@
       </c>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:7" ht="14.25">
+    <row r="10" spans="1:7" ht="13.8">
       <c r="A10" s="15" t="s">
         <v>21</v>
       </c>
@@ -997,10 +985,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>23</v>
@@ -1010,7 +998,7 @@
       </c>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:7" ht="14.25">
+    <row r="11" spans="1:7" ht="13.8">
       <c r="A11" s="27" t="s">
         <v>24</v>
       </c>
@@ -1018,10 +1006,10 @@
         <v>25</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>26</v>
@@ -1031,7 +1019,7 @@
       </c>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7" ht="14.25">
+    <row r="12" spans="1:7" ht="13.8">
       <c r="A12" s="15" t="s">
         <v>27</v>
       </c>
@@ -1039,10 +1027,10 @@
         <v>28</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>29</v>
@@ -1052,7 +1040,7 @@
       </c>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" ht="14.25">
+    <row r="13" spans="1:7" ht="13.8">
       <c r="A13" s="15" t="s">
         <v>41</v>
       </c>
@@ -1060,10 +1048,10 @@
         <v>38</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>30</v>
@@ -1073,7 +1061,7 @@
       </c>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7" ht="14.25">
+    <row r="14" spans="1:7" ht="13.8">
       <c r="A14" s="24" t="s">
         <v>42</v>
       </c>
@@ -1081,10 +1069,10 @@
         <v>43</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>44</v>
@@ -1094,7 +1082,7 @@
       </c>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" ht="14.25">
+    <row r="15" spans="1:7" ht="13.8">
       <c r="A15" s="15" t="s">
         <v>31</v>
       </c>
@@ -1102,10 +1090,10 @@
         <v>32</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>33</v>
@@ -1123,10 +1111,10 @@
         <v>35</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>36</v>
@@ -1138,35 +1126,37 @@
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="E17" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="F17" s="2">
         <v>1</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1">
       <c r="A18" s="30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>45</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>46</v>
@@ -1175,31 +1165,17 @@
         <v>1</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1">
-      <c r="A19" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="2">
-        <v>1</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>86</v>
-      </c>
+      <c r="A19" s="30"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="17"/>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1">
       <c r="A20" s="20"/>
@@ -1209,101 +1185,101 @@
       <c r="E20" s="10"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="1:7" ht="14.25">
+    <row r="21" spans="1:7" ht="13.8">
       <c r="A21" s="20"/>
     </row>
-    <row r="22" spans="1:7" ht="14.25">
+    <row r="22" spans="1:7" ht="13.8">
       <c r="A22" s="20"/>
     </row>
-    <row r="23" spans="1:7" ht="14.25">
+    <row r="23" spans="1:7" ht="13.8">
       <c r="A23" s="20"/>
     </row>
-    <row r="24" spans="1:7" ht="15">
+    <row r="24" spans="1:7" ht="14.4">
       <c r="A24" s="20"/>
       <c r="B24" s="22"/>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
       <c r="E24" s="13"/>
     </row>
-    <row r="25" spans="1:7" ht="15">
+    <row r="25" spans="1:7" ht="14.4">
       <c r="A25" s="20"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
     </row>
-    <row r="26" spans="1:7" ht="15">
+    <row r="26" spans="1:7" ht="14.4">
       <c r="B26" s="22"/>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
       <c r="E26" s="13"/>
     </row>
-    <row r="27" spans="1:7" ht="15">
+    <row r="27" spans="1:7" ht="14.4">
       <c r="B27" s="22"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
       <c r="E27" s="13"/>
     </row>
-    <row r="28" spans="1:7" ht="15">
+    <row r="28" spans="1:7" ht="14.4">
       <c r="B28" s="22"/>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
       <c r="E28" s="13"/>
     </row>
-    <row r="29" spans="1:7" ht="15">
+    <row r="29" spans="1:7" ht="14.4">
       <c r="B29" s="22"/>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
       <c r="E29" s="14"/>
     </row>
-    <row r="30" spans="1:7" ht="15">
+    <row r="30" spans="1:7" ht="14.4">
       <c r="B30" s="22"/>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
       <c r="E30" s="13"/>
     </row>
-    <row r="31" spans="1:7" ht="15">
+    <row r="31" spans="1:7" ht="14.4">
       <c r="B31" s="22"/>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
       <c r="E31" s="13"/>
     </row>
-    <row r="32" spans="1:7" ht="15">
+    <row r="32" spans="1:7" ht="14.4">
       <c r="B32" s="22"/>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
       <c r="E32" s="13"/>
     </row>
-    <row r="33" spans="2:5" ht="15">
+    <row r="33" spans="2:5" ht="14.4">
       <c r="B33" s="22"/>
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
       <c r="E33" s="13"/>
     </row>
-    <row r="34" spans="2:5" ht="15">
+    <row r="34" spans="2:5" ht="14.4">
       <c r="B34" s="22"/>
       <c r="C34" s="26"/>
       <c r="D34" s="26"/>
       <c r="E34" s="13"/>
     </row>
-    <row r="35" spans="2:5" ht="15">
+    <row r="35" spans="2:5" ht="14.4">
       <c r="B35" s="22"/>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
       <c r="E35" s="13"/>
     </row>
-    <row r="36" spans="2:5" ht="15">
+    <row r="36" spans="2:5" ht="14.4">
       <c r="B36" s="22"/>
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
       <c r="E36" s="13"/>
     </row>
-    <row r="37" spans="2:5" ht="15">
+    <row r="37" spans="2:5" ht="14.4">
       <c r="B37" s="22"/>
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
       <c r="E37" s="13"/>
     </row>
-    <row r="38" spans="2:5" ht="15">
+    <row r="38" spans="2:5" ht="14.4">
       <c r="B38" s="22"/>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
@@ -1325,10 +1301,9 @@
     <hyperlink ref="E16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="E13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="E14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E19" r:id="rId15" xr:uid="{AF70850A-D00A-5245-BD95-498486583EB1}"/>
-    <hyperlink ref="E18" r:id="rId16" xr:uid="{94E5A8C3-78A8-9440-B662-5AF496B52542}"/>
+    <hyperlink ref="E18" r:id="rId15" xr:uid="{94E5A8C3-78A8-9440-B662-5AF496B52542}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>